<commit_message>
final version before sending
</commit_message>
<xml_diff>
--- a/thesis/resources/toc.xlsx
+++ b/thesis/resources/toc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\mgr\thesis\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667B9BD7-E55D-41F3-AEBB-ED51A1616865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF5DD84-C05D-45CF-B132-B3D75408FCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{9ABD2D86-3B99-44F9-BC5C-8F2CE1D9E2FC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>Summary</t>
   </si>
@@ -99,21 +99,12 @@
     <t>References</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>2.1</t>
   </si>
   <si>
     <t>2.2</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -126,27 +117,15 @@
     <t>12</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
     <t>4.2</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>4.3</t>
   </si>
   <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
     <t>5.1</t>
   </si>
   <si>
@@ -159,9 +138,6 @@
     <t>5.3</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>52</t>
   </si>
   <si>
@@ -174,9 +150,6 @@
     <t>59</t>
   </si>
   <si>
-    <t>61</t>
-  </si>
-  <si>
     <t>CHAPTER I.</t>
   </si>
   <si>
@@ -196,6 +169,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>60</t>
   </si>
 </sst>
 </file>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADB91C7-5332-497F-83B7-AA13F4521781}">
   <dimension ref="A8:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -597,16 +597,16 @@
   <sheetData>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1" t="str">
         <f>A8&amp;B8&amp;C8</f>
@@ -616,49 +616,48 @@
         <f>F8&amp;H8</f>
         <v>CHAPTER I. Introduction</v>
       </c>
-      <c r="K8" s="5" t="str">
-        <f>D8</f>
-        <v>2</v>
+      <c r="K8" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H9" s="1" t="str">
         <f t="shared" ref="H9:H28" si="0">A9&amp;B9&amp;C9</f>
         <v xml:space="preserve"> Literature review</v>
       </c>
       <c r="J9" s="4" t="str">
-        <f t="shared" ref="J9:J28" si="1">F9&amp;H9</f>
+        <f t="shared" ref="J9:J27" si="1">F9&amp;H9</f>
         <v>CHAPTER II. Literature review</v>
       </c>
       <c r="K9" s="5" t="str">
         <f t="shared" ref="K9:K28" si="2">D9</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="H10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -670,21 +669,21 @@
       </c>
       <c r="K10" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -696,12 +695,12 @@
       </c>
       <c r="K11" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
@@ -710,7 +709,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -722,15 +721,15 @@
       </c>
       <c r="K12" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -748,21 +747,21 @@
       </c>
       <c r="K13" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="H14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -774,21 +773,21 @@
       </c>
       <c r="K14" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -800,21 +799,21 @@
       </c>
       <c r="K15" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -826,21 +825,21 @@
       </c>
       <c r="K16" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="H17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -852,21 +851,21 @@
       </c>
       <c r="K17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -878,73 +877,73 @@
       </c>
       <c r="K18" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Results</v>
+      </c>
+      <c r="J19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CHAPTER V. Results</v>
+      </c>
+      <c r="K19" s="5" t="str">
+        <f t="shared" si="2"/>
         <v>36</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> Results</v>
-      </c>
-      <c r="J19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>CHAPTER V. Results</v>
-      </c>
-      <c r="K19" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>5.1. Results of the pre-modeling phase</v>
+      </c>
+      <c r="J20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>5.1. Results of the pre-modeling phase</v>
+      </c>
+      <c r="K20" s="5" t="str">
+        <f t="shared" si="2"/>
         <v>36</v>
-      </c>
-      <c r="H20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>5.1. Results of the pre-modeling phase</v>
-      </c>
-      <c r="J20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>5.1. Results of the pre-modeling phase</v>
-      </c>
-      <c r="K20" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -956,21 +955,21 @@
       </c>
       <c r="K21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -982,21 +981,21 @@
       </c>
       <c r="K22" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1016,7 +1015,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1036,7 +1035,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1056,7 +1055,7 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1076,7 +1075,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1096,7 +1095,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1108,7 +1107,7 @@
       </c>
       <c r="K28" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>